<commit_message>
replaced relays with n-channel fets
</commit_message>
<xml_diff>
--- a/p.xlsx
+++ b/p.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick Chau\Documents\GitHub\Racing-Fuses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB4E9A5-92CB-47E1-A81D-C1AF3AD03D71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24ADC3D3-80A8-40AA-9D31-BB43C7C63932}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{78198D8F-48C7-4936-8318-FF0E53B3794D}"/>
   </bookViews>
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>https://www.digikey.com/product-detail/en/mpd-memory-protection-devices/BK-6010/BK-6010-ND/2330529</t>
   </si>
   <si>
-    <t>IRLB8721PbF</t>
-  </si>
-  <si>
     <t>https://www.nteinc.com/specs/original/BC558.pdf</t>
   </si>
   <si>
@@ -71,24 +68,12 @@
     <t>Blown Fuse Diode</t>
   </si>
   <si>
-    <t>510 Ohm Resistor</t>
-  </si>
-  <si>
-    <t>510K Ohm Resistor</t>
-  </si>
-  <si>
     <t>1N4148</t>
   </si>
   <si>
     <t>https://www.vishay.com/docs/81857/1n4148.pdf</t>
   </si>
   <si>
-    <t>8MHz Clock</t>
-  </si>
-  <si>
-    <t>https://datasheets.maximintegrated.com/en/ds/MAX7375.pdf</t>
-  </si>
-  <si>
     <t>Teensy 3.2</t>
   </si>
   <si>
@@ -102,6 +87,54 @@
   </si>
   <si>
     <t>BK-6010</t>
+  </si>
+  <si>
+    <t>https://assets.nexperia.com/documents/data-sheet/BUK9Y12-40E.pdf</t>
+  </si>
+  <si>
+    <t>BUK9Y12-40E</t>
+  </si>
+  <si>
+    <t>Necessary Inputs</t>
+  </si>
+  <si>
+    <t>BATT+</t>
+  </si>
+  <si>
+    <t>BATT GND</t>
+  </si>
+  <si>
+    <t>EFI_MAIN_SIG</t>
+  </si>
+  <si>
+    <t>PUMP_SIG</t>
+  </si>
+  <si>
+    <t>FAN_SIG</t>
+  </si>
+  <si>
+    <t>INJ_SIG</t>
+  </si>
+  <si>
+    <t>COIL_SIG</t>
+  </si>
+  <si>
+    <t>CANH</t>
+  </si>
+  <si>
+    <t>CANL</t>
+  </si>
+  <si>
+    <t>AUX</t>
+  </si>
+  <si>
+    <t>AUX_2</t>
+  </si>
+  <si>
+    <t>DIR</t>
+  </si>
+  <si>
+    <t>O2</t>
   </si>
 </sst>
 </file>
@@ -473,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A67C9C-1F23-4D41-8CEA-5F19B96D76CA}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -488,24 +521,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>0</v>
@@ -513,66 +546,119 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" t="s">
-        <v>17</v>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>